<commit_message>
Fixed issue with Analytics not working
</commit_message>
<xml_diff>
--- a/src/ADAM.xlsx
+++ b/src/ADAM.xlsx
@@ -1,16 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26405"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3DF0F42-7440-4699-A448-FE1F5BB49845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADAM_MBM_Worked" sheetId="1" r:id="rId1"/>
     <sheet name="ADAM_UET_Worked" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -23,6 +37,9 @@
     <t>Action</t>
   </si>
   <si>
+    <t>Automatically Assigned Ticket</t>
+  </si>
+  <si>
     <t>09:53:12 01-23-2023</t>
   </si>
   <si>
@@ -107,6 +124,9 @@
     <t>08:32:21 03-23-2023</t>
   </si>
   <si>
+    <t>Manually Assigned Ticket</t>
+  </si>
+  <si>
     <t>08:31:40 03-24-2023</t>
   </si>
   <si>
@@ -179,12 +199,6 @@
     <t>18:55:07 04-11-2023</t>
   </si>
   <si>
-    <t>Automatically Assigned Ticket</t>
-  </si>
-  <si>
-    <t>Manually Assigned Ticket</t>
-  </si>
-  <si>
     <t>ADAM_UET_Worked</t>
   </si>
   <si>
@@ -209,18 +223,18 @@
     <t>20:54:09 04-11-2023</t>
   </si>
   <si>
+    <t>Ticket Assignment Undone @ 10:09:16 04-12-2023</t>
+  </si>
+  <si>
     <t>12:10:10 04-12-2023</t>
-  </si>
-  <si>
-    <t>Ticket Assignment Undone @ 10:09:16 04-12-2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -286,6 +300,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -332,7 +354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,9 +386,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,6 +438,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -573,12 +631,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G58" sqref="A56:G58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -590,434 +653,434 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>44943.41357638889</v>
+        <v>44943.413576388892</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>44943.628125</v>
+        <v>44943.628125000003</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1026,12 +1089,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -1046,7 +1112,7 @@
         <v>44939.67863425926</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1054,7 +1120,7 @@
         <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1062,7 +1128,7 @@
         <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1070,7 +1136,7 @@
         <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1078,7 +1144,7 @@
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1086,7 +1152,7 @@
         <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1094,7 +1160,7 @@
         <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1102,15 +1168,15 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>